<commit_message>
added thermister stuff to BOM
</commit_message>
<xml_diff>
--- a/Documentation/BOM.xlsx
+++ b/Documentation/BOM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -63,13 +63,16 @@
     <t xml:space="preserve">Battery</t>
   </si>
   <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
     <t xml:space="preserve">n/A</t>
   </si>
   <si>
     <t xml:space="preserve">C1-C4</t>
   </si>
   <si>
-    <t xml:space="preserve">10uf</t>
+    <t xml:space="preserve">10u</t>
   </si>
   <si>
     <t xml:space="preserve">C19702</t>
@@ -174,7 +177,7 @@
     <t xml:space="preserve">C5</t>
   </si>
   <si>
-    <t xml:space="preserve">1uf</t>
+    <t xml:space="preserve">1u</t>
   </si>
   <si>
     <t xml:space="preserve">C52923</t>
@@ -195,6 +198,18 @@
     <t xml:space="preserve">0402WGF8201TCE</t>
   </si>
   <si>
+    <t xml:space="preserve">R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402WGF100KTCE</t>
+  </si>
+  <si>
     <t xml:space="preserve">RV1</t>
   </si>
   <si>
@@ -205,6 +220,18 @@
   </si>
   <si>
     <t xml:space="preserve">RK09K1130AJ3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100k Thermister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C77130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCP15WF104F03RC</t>
   </si>
   <si>
     <t xml:space="preserve">U6</t>
@@ -226,9 +253,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.0000;[RED]\-[$$-409]#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -324,7 +352,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -359,6 +387,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -494,14 +526,14 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.61"/>
@@ -551,15 +583,17 @@
         <v>11</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>0</v>
@@ -574,10 +608,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -585,10 +619,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>0.0066</v>
@@ -603,10 +637,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -614,10 +648,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>0.0119</v>
@@ -632,10 +666,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -643,10 +677,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>0.0054</v>
@@ -661,10 +695,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -672,10 +706,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H6" s="5" t="n">
         <v>0.001</v>
@@ -690,10 +724,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -701,10 +735,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>0.001</v>
@@ -719,10 +753,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -730,10 +764,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H8" s="5" t="n">
         <v>0.001</v>
@@ -748,10 +782,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -759,10 +793,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H9" s="3" t="n">
         <v>0.0333</v>
@@ -777,10 +811,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -788,10 +822,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>0.2027</v>
@@ -806,10 +840,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -817,10 +851,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>0.0725</v>
@@ -835,10 +869,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -846,10 +880,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>0.478</v>
@@ -871,7 +905,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J13" s="7" t="n">
         <f aca="false">SUM(power_componentes[Total cost (5 Boards)])</f>
@@ -903,7 +937,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -953,23 +987,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.33"/>
   </cols>
   <sheetData>
@@ -1007,19 +1041,19 @@
     </row>
     <row r="2" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>0.0038</v>
@@ -1034,19 +1068,19 @@
     </row>
     <row r="3" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H3" s="5" t="n">
         <v>0.0005</v>
@@ -1059,41 +1093,38 @@
         <v>0.0075</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>56</v>
+    <row r="4" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>0.5956</v>
+        <v>0.0007</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J4" s="5" t="n">
         <f aca="false">H4*E4*5+I4</f>
-        <v>5.978</v>
+        <v>0.0035</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E5" s="0" t="n">
@@ -1106,24 +1137,81 @@
         <v>64</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>0.3887</v>
+        <v>0.5956</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>3</v>
       </c>
       <c r="J5" s="5" t="n">
         <f aca="false">H5*E5*5+I5</f>
+        <v>5.978</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0.0131</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <f aca="false">H6*E6*5+I6</f>
+        <v>3.0655</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>0.3887</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <f aca="false">H7*E7*5+I7</f>
         <v>4.9435</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H6" s="5"/>
-      <c r="I6" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="9" t="n">
-        <f aca="false">SUM(J2:J5)</f>
-        <v>10.948</v>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="5"/>
+      <c r="I8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="10" t="n">
+        <f aca="false">SUM(J2:J7)</f>
+        <v>14.017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>